<commit_message>
14.05 Added loader for BGR stratigraphy and updated BGE-SV loader.
</commit_message>
<xml_diff>
--- a/055689800201_Wagenhoff-2_GeolProfile.xlsx
+++ b/055689800201_Wagenhoff-2_GeolProfile.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://terrageoservice.sharepoint.com/sites/BGRWarm-Up/Shared Documents/04_BGR Data Exchange/well_data/05568980020_Wagenhoff-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suess/PythonProject/PyQTWellSection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{6E3EC78C-8610-4188-A0E4-A7BFDA366AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBDCB749-C512-934E-ADD1-F3AFFDD219E1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0853C4-93C3-6E4B-B469-F95D2C3E4890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RWE_Dea-DEA-WinDEA" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -609,7 +608,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard_RWE_Dea-DEA-WinDEA" xfId="1" xr:uid="{9DE82CD3-24FB-4F3D-B735-0EBE6D3860DB}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -890,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -5713,19 +5712,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7860DC0D-CF63-C24C-A40A-4989EAA6C624}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1367417c-9185-4bd3-948f-46c1009b254f">
@@ -5734,15 +5730,6 @@
     <TaxCatchAll xmlns="9d0de0af-308b-4838-8022-b97f48424173" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5935,6 +5922,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DFC0395-9C56-44AD-BC92-C0E4F23A76E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{779039E0-F034-474B-BB79-23D34831C4CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5951,14 +5946,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DFC0395-9C56-44AD-BC92-C0E4F23A76E4}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B341C6B-2D2A-41EA-BE9C-5E830B8ED6DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1367417c-9185-4bd3-948f-46c1009b254f"/>
+    <ds:schemaRef ds:uri="9d0de0af-308b-4838-8022-b97f48424173"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B341C6B-2D2A-41EA-BE9C-5E830B8ED6DF}"/>
 </file>
</xml_diff>